<commit_message>
działa - wyniki raz są ok, raz nie ok
</commit_message>
<xml_diff>
--- a/analiza_wag_szczegolowa.xlsx
+++ b/analiza_wag_szczegolowa.xlsx
@@ -519,32 +519,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(128, 70)</t>
+          <t>(256, 70)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8960</v>
+        <v>17920</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01660643331706524</v>
+        <v>-0.01711405254900455</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2210999429225922</v>
+        <v>0.1603449732065201</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.9853721261024475</v>
+        <v>-0.7438752055168152</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8720182776451111</v>
+        <v>0.695008397102356</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.007439462468028069</v>
+        <v>-0.008567610755562782</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.1387902796268463</v>
+        <v>-0.1068862080574036</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1055527850985527</v>
+        <v>0.07274356484413147</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -553,11 +553,11 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1.857390403747559</v>
+        <v>1.438883543014526</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.5237723214285714), 'positive_ratio': np.float64(0.47622767857142856), 'near_zero_ratio': np.float64(0.4390625)}</t>
+          <t>{'negative_ratio': np.float64(0.5322544642857143), 'positive_ratio': np.float64(0.46774553571428573), 'near_zero_ratio': np.float64(0.5361049107142857)}</t>
         </is>
       </c>
     </row>
@@ -569,45 +569,45 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(64, 128)</t>
+          <t>(128, 256)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8192</v>
+        <v>32768</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.113348662853241</v>
+        <v>-0.05280745029449463</v>
       </c>
       <c r="E3" t="n">
-        <v>0.270563542842865</v>
+        <v>0.1543912589550018</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.623992443084717</v>
+        <v>-1.139596462249756</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7208037972450256</v>
+        <v>0.5488262176513672</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.02865528129041195</v>
+        <v>-0.01943532377481461</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.2314581722021103</v>
+        <v>-0.1248481050133705</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05673712491989136</v>
+        <v>0.04602491855621338</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L3" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="M3" t="n">
-        <v>2.344796180725098</v>
+        <v>1.688422679901123</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.578857421875), 'positive_ratio': np.float64(0.421142578125), 'near_zero_ratio': np.float64(0.4761962890625)}</t>
+          <t>{'negative_ratio': np.float64(0.57470703125), 'positive_ratio': np.float64(0.42529296875), 'near_zero_ratio': np.float64(0.597869873046875)}</t>
         </is>
       </c>
     </row>
@@ -619,45 +619,45 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(32, 64)</t>
+          <t>(64, 128)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.109308123588562</v>
+        <v>-0.08466237783432007</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2775891423225403</v>
+        <v>0.1818512678146362</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.313855290412903</v>
+        <v>-1.142301201820374</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8337620496749878</v>
+        <v>0.7446489334106445</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.03686981648206711</v>
+        <v>-0.03681820631027222</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.2830344140529633</v>
+        <v>-0.2019456475973129</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06253048032522202</v>
+        <v>0.03562135994434357</v>
       </c>
       <c r="K4" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>2.147617340087891</v>
+        <v>1.886950135231018</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.5869140625), 'positive_ratio': np.float64(0.4130859375), 'near_zero_ratio': np.float64(0.39794921875)}</t>
+          <t>{'negative_ratio': np.float64(0.620361328125), 'positive_ratio': np.float64(0.379638671875), 'near_zero_ratio': np.float64(0.5172119140625)}</t>
         </is>
       </c>
     </row>
@@ -669,32 +669,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(2, 32)</t>
+          <t>(2, 64)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D5" t="n">
-        <v>0.005295651964843273</v>
+        <v>-0.0002197984140366316</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1508176177740097</v>
+        <v>0.1146299988031387</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.275058776140213</v>
+        <v>-0.2582334876060486</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5613259077072144</v>
+        <v>0.2840132713317871</v>
       </c>
       <c r="H5" t="n">
-        <v>0.00798221118748188</v>
+        <v>0.008058508858084679</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.1098269820213318</v>
+        <v>-0.1018093079328537</v>
       </c>
       <c r="J5" t="n">
-        <v>0.116675853729248</v>
+        <v>0.09006457775831223</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -703,11 +703,11 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.836384654045105</v>
+        <v>0.5422467589378357</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.46875), 'positive_ratio': np.float64(0.53125), 'near_zero_ratio': np.float64(0.359375)}</t>
+          <t>{'negative_ratio': np.float64(0.46875), 'positive_ratio': np.float64(0.53125), 'near_zero_ratio': np.float64(0.53125)}</t>
         </is>
       </c>
     </row>
@@ -810,45 +810,45 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(128, 70)</t>
+          <t>(256, 70)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8960</v>
+        <v>17920</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01089047361165285</v>
+        <v>-0.008874831721186638</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1639692634344101</v>
+        <v>0.1233037412166595</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.8420926928520203</v>
+        <v>-0.7738926410675049</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6090128421783447</v>
+        <v>0.4860520660877228</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.004111271351575851</v>
+        <v>-0.004700297489762306</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.09759660065174103</v>
+        <v>-0.07732301950454712</v>
       </c>
       <c r="J2" t="n">
-        <v>0.07543257623910904</v>
+        <v>0.05924554169178009</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1.45110559463501</v>
+        <v>1.259944677352905</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.5198660714285714), 'positive_ratio': np.float64(0.48013392857142856), 'near_zero_ratio': np.float64(0.5401785714285714)}</t>
+          <t>{'negative_ratio': np.float64(0.52421875), 'positive_ratio': np.float64(0.47578125), 'near_zero_ratio': np.float64(0.6307477678571428)}</t>
         </is>
       </c>
     </row>
@@ -860,45 +860,45 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(64, 128)</t>
+          <t>(128, 256)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8192</v>
+        <v>32768</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1030008345842361</v>
+        <v>-0.05243252962827682</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2501073777675629</v>
+        <v>0.1463489234447479</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.583622694015503</v>
+        <v>-0.9223895072937012</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7201523184776306</v>
+        <v>0.5513448119163513</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.01735761947929859</v>
+        <v>-0.01403271965682507</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.1894769668579102</v>
+        <v>-0.1144021451473236</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04702752828598022</v>
+        <v>0.04133421182632446</v>
       </c>
       <c r="K3" t="n">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="L3" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>2.303775072097778</v>
+        <v>1.473734378814697</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.5616455078125), 'positive_ratio': np.float64(0.4383544921875), 'near_zero_ratio': np.float64(0.5462646484375)}</t>
+          <t>{'negative_ratio': np.float64(0.56787109375), 'positive_ratio': np.float64(0.43212890625), 'near_zero_ratio': np.float64(0.6468505859375)}</t>
         </is>
       </c>
     </row>
@@ -910,45 +910,45 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(32, 64)</t>
+          <t>(64, 128)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.09833788126707077</v>
+        <v>-0.07360292971134186</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2478403747081757</v>
+        <v>0.16595458984375</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.042535185813904</v>
+        <v>-0.7039116621017456</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8181487917900085</v>
+        <v>0.5289499759674072</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.04238573461771011</v>
+        <v>-0.03143126145005226</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.2619812190532684</v>
+        <v>-0.1800456941127777</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06465944647789001</v>
+        <v>0.03734163194894791</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>1.860683917999268</v>
+        <v>1.232861638069153</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.59619140625), 'positive_ratio': np.float64(0.40380859375), 'near_zero_ratio': np.float64(0.4111328125)}</t>
+          <t>{'negative_ratio': np.float64(0.60888671875), 'positive_ratio': np.float64(0.39111328125), 'near_zero_ratio': np.float64(0.5406494140625)}</t>
         </is>
       </c>
     </row>
@@ -960,32 +960,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(2, 32)</t>
+          <t>(2, 64)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02888038009405136</v>
+        <v>-0.0008837929926812649</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1967049837112427</v>
+        <v>0.1321490854024887</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.4117404222488403</v>
+        <v>-0.3066065013408661</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3668105900287628</v>
+        <v>0.2701490223407745</v>
       </c>
       <c r="H5" t="n">
-        <v>0.066961869597435</v>
+        <v>0.01635450311005116</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.1443266868591309</v>
+        <v>-0.1083608865737915</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1863077282905579</v>
+        <v>0.1086637452244759</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -994,11 +994,11 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7785509824752808</v>
+        <v>0.5767555236816406</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{'negative_ratio': np.float64(0.4375), 'positive_ratio': np.float64(0.5625), 'near_zero_ratio': np.float64(0.265625)}</t>
+          <t>{'negative_ratio': np.float64(0.46875), 'positive_ratio': np.float64(0.53125), 'near_zero_ratio': np.float64(0.4140625)}</t>
         </is>
       </c>
     </row>
@@ -1076,26 +1076,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(128,)</t>
+          <t>(256,)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.7857880592346191</v>
+        <v>-0.5612590909004211</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3125021159648895</v>
+        <v>0.2049462050199509</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.483299136161804</v>
+        <v>-1.172370314598083</v>
       </c>
       <c r="G2" t="n">
-        <v>0.118424117565155</v>
+        <v>-0.01639115251600742</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.786268413066864</v>
+        <v>-0.5743221044540405</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1109,26 +1109,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(64,)</t>
+          <t>(128,)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1600780189037323</v>
+        <v>0.00926684308797121</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4534048140048981</v>
+        <v>0.3524489104747772</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.054399728775024</v>
+        <v>-1.096748352050781</v>
       </c>
       <c r="G3" t="n">
-        <v>1.085022211074829</v>
+        <v>0.7321162819862366</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2179315388202667</v>
+        <v>0.03953400254249573</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1142,26 +1142,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(32,)</t>
+          <t>(64,)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D4" t="n">
-        <v>0.401515007019043</v>
+        <v>0.445732593536377</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3000015318393707</v>
+        <v>0.08467815816402435</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.150766730308533</v>
+        <v>0.2514960467815399</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7201817631721497</v>
+        <v>0.6003814935684204</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4576926529407501</v>
+        <v>0.4430473446846008</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1182,19 +1182,19 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.08950012922286987</v>
+        <v>-0.08648733794689178</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05255741998553276</v>
+        <v>0.0126589797437191</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1420575529336929</v>
+        <v>-0.09914632141590118</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.03694271296262741</v>
+        <v>-0.07382836192846298</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.08950012922286987</v>
+        <v>-0.08648733794689178</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1274,26 +1274,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(128,)</t>
+          <t>(256,)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.6339899301528931</v>
+        <v>-0.3838124871253967</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2155577540397644</v>
+        <v>0.134968176484108</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.239803075790405</v>
+        <v>-0.7661592364311218</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.1035583838820457</v>
+        <v>0.05474037304520607</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.6350626945495605</v>
+        <v>-0.3820775151252747</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1307,26 +1307,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(64,)</t>
+          <t>(128,)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05864047631621361</v>
+        <v>0.02567333169281483</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3848187327384949</v>
+        <v>0.2512891590595245</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.6931341886520386</v>
+        <v>-0.5473055839538574</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8018662333488464</v>
+        <v>0.7028363943099976</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08350060135126114</v>
+        <v>0.001539497869089246</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1340,26 +1340,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(32,)</t>
+          <t>(64,)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2686272859573364</v>
+        <v>0.3147733211517334</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1167903691530228</v>
+        <v>0.1046170219779015</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.08565711975097656</v>
+        <v>0.02957485429942608</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4241971075534821</v>
+        <v>0.533165454864502</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3039396405220032</v>
+        <v>0.3192217648029327</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1380,19 +1380,19 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1752697080373764</v>
+        <v>-0.1392880976200104</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0343460738658905</v>
+        <v>0.01767654344439507</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2096157819032669</v>
+        <v>-0.1569646447896957</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1409236341714859</v>
+        <v>-0.1216115579009056</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.1752697080373764</v>
+        <v>-0.1392880976200104</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1441,75 +1441,75 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2407293319702148</v>
+        <v>0.1594968289136887</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8896910548210144</v>
+        <v>0.7483857870101929</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>data__tagData__linearAcceleration__x</t>
+          <t>data__tagData__quaternion__x</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2227869182825089</v>
+        <v>0.1507901549339294</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8233792185783386</v>
+        <v>0.7075326442718506</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__y</t>
+          <t>data__tagData__linearAcceleration__x</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2164704352617264</v>
+        <v>0.1438106447458267</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8000346422195435</v>
+        <v>0.6747835874557495</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>data__tagData__magnetic__x</t>
+          <t>data__tagData__quaternion__y</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2005293667316437</v>
+        <v>0.1433026343584061</v>
       </c>
       <c r="C5" t="n">
-        <v>0.741119384765625</v>
+        <v>0.6723999381065369</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__x</t>
+          <t>data__tagData__magnetic__x</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1963941305875778</v>
+        <v>0.1378122717142105</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7258363366127014</v>
+        <v>0.6466382145881653</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>data__tagData__pressure</t>
+          <t>data__tagData__quaternion__z</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1881137788295746</v>
+        <v>0.1320609897375107</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6952337026596069</v>
+        <v>0.619652271270752</v>
       </c>
     </row>
     <row r="8">
@@ -1519,36 +1519,36 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1785637140274048</v>
+        <v>0.1298420280218124</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6599383950233459</v>
+        <v>0.6092405319213867</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__z</t>
+          <t>data__tagData__quaternion__w</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1723896265029907</v>
+        <v>0.1210319921374321</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6371201276779175</v>
+        <v>0.5679023265838623</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__w</t>
+          <t>data__tagData__pressure</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1489551514387131</v>
+        <v>0.1203977465629578</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5505106449127197</v>
+        <v>0.5649263858795166</v>
       </c>
     </row>
     <row r="11">
@@ -1558,36 +1558,36 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1459620594978333</v>
+        <v>0.1117235496640205</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5394487380981445</v>
+        <v>0.5242255926132202</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>data__tagData__linearAcceleration__z</t>
+          <t>data__tagData__gyro__z</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1034700945019722</v>
+        <v>0.06795907020568848</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3824062943458557</v>
+        <v>0.3188753128051758</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>data__tagData__gyro__z</t>
+          <t>data__tagData__linearAcceleration__z</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.08689176291227341</v>
+        <v>0.06748020648956299</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3211358785629272</v>
+        <v>0.3166284263134003</v>
       </c>
     </row>
     <row r="14">
@@ -1597,10 +1597,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.04890290647745132</v>
+        <v>0.0470699667930603</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1807360798120499</v>
+        <v>0.2208601534366608</v>
       </c>
     </row>
     <row r="15">
@@ -1610,10 +1610,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.03741945698857307</v>
+        <v>0.04119820147752762</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1382953822612762</v>
+        <v>0.1933088600635529</v>
       </c>
     </row>
   </sheetData>
@@ -1655,53 +1655,53 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__x</t>
+          <t>data__tagData__magnetic__z</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1686586290597916</v>
+        <v>0.1268749982118607</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8205990195274353</v>
+        <v>0.7880849838256836</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>data__tagData__magnetic__z</t>
+          <t>data__tagData__quaternion__x</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1676810681819916</v>
+        <v>0.1235200688242912</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8158428072929382</v>
+        <v>0.7672458291053772</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__y</t>
+          <t>data__tagData__magnetic__x</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1590362042188644</v>
+        <v>0.1187189370393753</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7737816572189331</v>
+        <v>0.7374235391616821</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>data__tagData__pressure</t>
+          <t>data__tagData__quaternion__y</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.151473730802536</v>
+        <v>0.1174513921141624</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7369868755340576</v>
+        <v>0.7295501828193665</v>
       </c>
     </row>
     <row r="6">
@@ -1711,62 +1711,62 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1499738693237305</v>
+        <v>0.1046234965324402</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7296894192695618</v>
+        <v>0.6498696208000183</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>data__tagData__magnetic__x</t>
+          <t>data__tagData__pressure</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1496226489543915</v>
+        <v>0.1025804728269577</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7279805541038513</v>
+        <v>0.6371793746948242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>data__tagData__magnetic__y</t>
+          <t>data__tagData__linearAcceleration__y</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1439113020896912</v>
+        <v>0.09987609833478928</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7001923322677612</v>
+        <v>0.6203811168670654</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>data__tagData__quaternion__z</t>
+          <t>data__tagData__magnetic__y</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1395293325185776</v>
+        <v>0.09966656565666199</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6788721084594727</v>
+        <v>0.61907958984375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>data__tagData__linearAcceleration__y</t>
+          <t>data__tagData__quaternion__z</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1232196167111397</v>
+        <v>0.09737355262041092</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5995181202888489</v>
+        <v>0.6048365235328674</v>
       </c>
     </row>
     <row r="11">
@@ -1776,10 +1776,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1208132654428482</v>
+        <v>0.08796892315149307</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5878100991249084</v>
+        <v>0.546419620513916</v>
       </c>
     </row>
     <row r="12">
@@ -1789,36 +1789,36 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.08199863880872726</v>
+        <v>0.07794170081615448</v>
       </c>
       <c r="C12" t="n">
-        <v>0.398959755897522</v>
+        <v>0.4841354489326477</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>data__tagData__gyro__y</t>
+          <t>data__tagData__gyro__z</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.02548693493008614</v>
+        <v>0.02600033208727837</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1240052431821823</v>
+        <v>0.1615012586116791</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>data__tagData__gyro__z</t>
+          <t>data__tagData__gyro__y</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02124491706490517</v>
+        <v>0.02569006010890007</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1033659428358078</v>
+        <v>0.1595740020275116</v>
       </c>
     </row>
     <row r="15">
@@ -1828,10 +1828,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.02068973705172539</v>
+        <v>0.02475104667246342</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1006647497415543</v>
+        <v>0.1537413001060486</v>
       </c>
     </row>
   </sheetData>
@@ -1912,31 +1912,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01660643331706524</v>
+        <v>-0.01711405254900455</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01089047361165285</v>
+        <v>-0.008874831721186638</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005715959705412388</v>
+        <v>0.008239220827817917</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2210999429225922</v>
+        <v>0.1603449732065201</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1639692634344101</v>
+        <v>0.1233037412166595</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.05713067948818207</v>
+        <v>-0.03704123198986053</v>
       </c>
       <c r="H2" t="n">
-        <v>1.857390403747559</v>
+        <v>1.438883543014526</v>
       </c>
       <c r="I2" t="n">
-        <v>1.45110559463501</v>
+        <v>1.259944677352905</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.4062848091125488</v>
+        <v>-0.1789388656616211</v>
       </c>
     </row>
     <row r="3">
@@ -1946,31 +1946,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.113348662853241</v>
+        <v>-0.05280745029449463</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1030008345842361</v>
+        <v>-0.05243252962827682</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01034782826900482</v>
+        <v>0.000374920666217804</v>
       </c>
       <c r="E3" t="n">
-        <v>0.270563542842865</v>
+        <v>0.1543912589550018</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2501073777675629</v>
+        <v>0.1463489234447479</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.02045616507530212</v>
+        <v>-0.008042335510253906</v>
       </c>
       <c r="H3" t="n">
-        <v>2.344796180725098</v>
+        <v>1.688422679901123</v>
       </c>
       <c r="I3" t="n">
-        <v>2.303775072097778</v>
+        <v>1.473734378814697</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.04102110862731934</v>
+        <v>-0.2146883010864258</v>
       </c>
     </row>
     <row r="4">
@@ -1980,31 +1980,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.109308123588562</v>
+        <v>-0.08466237783432007</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.09833788126707077</v>
+        <v>-0.07360292971134186</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01097024232149124</v>
+        <v>0.01105944812297821</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2775891423225403</v>
+        <v>0.1818512678146362</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2478403747081757</v>
+        <v>0.16595458984375</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.02974876761436462</v>
+        <v>-0.01589667797088623</v>
       </c>
       <c r="H4" t="n">
-        <v>2.147617340087891</v>
+        <v>1.886950135231018</v>
       </c>
       <c r="I4" t="n">
-        <v>1.860683917999268</v>
+        <v>1.232861638069153</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.286933422088623</v>
+        <v>-0.6540884971618652</v>
       </c>
     </row>
     <row r="5">
@@ -2014,31 +2014,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.005295651964843273</v>
+        <v>-0.0002197984140366316</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02888038009405136</v>
+        <v>-0.0008837929926812649</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02358472719788551</v>
+        <v>-0.0006639945786446333</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1508176177740097</v>
+        <v>0.1146299988031387</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1967049837112427</v>
+        <v>0.1321490854024887</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04588736593723297</v>
+        <v>0.01751908659934998</v>
       </c>
       <c r="H5" t="n">
-        <v>0.836384654045105</v>
+        <v>0.5422467589378357</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7785509824752808</v>
+        <v>0.5767555236816406</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.05783367156982422</v>
+        <v>0.03450876474380493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>